<commit_message>
add more matched institutions
</commit_message>
<xml_diff>
--- a/data/processed/leiden_matching_table.xlsx
+++ b/data/processed/leiden_matching_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tklebel\Documents\Projects\ON-MERRIT\03-Analysis\apc_effect\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81E17CD-6463-4173-A548-2384D1370E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C920C544-2CDE-4D19-A79D-0722E00546AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16354" yWindow="7646" windowWidth="22149" windowHeight="12103" xr2:uid="{70655950-438C-47E9-B52C-924540BD7C84}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="848">
   <si>
     <t>University</t>
   </si>
@@ -2116,6 +2116,489 @@
   </si>
   <si>
     <t>NL</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I182083151</t>
+  </si>
+  <si>
+    <t>King Juan Carlos University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I904495901</t>
+  </si>
+  <si>
+    <t>Ruhr University Bochum</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I172901346</t>
+  </si>
+  <si>
+    <t>St Petersburg University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I227306068</t>
+  </si>
+  <si>
+    <t>Ondokuz Mayıs University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I878213199</t>
+  </si>
+  <si>
+    <t>University of Pune</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I196051555</t>
+  </si>
+  <si>
+    <t>Shahid Chamran University of Ahvaz</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I194604659</t>
+  </si>
+  <si>
+    <t>Shiraz University of Medical Sciences</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I47838141</t>
+  </si>
+  <si>
+    <t>Saint Louis University</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I59553526</t>
+  </si>
+  <si>
+    <t>Stony Brook University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I174306211</t>
+  </si>
+  <si>
+    <t>Technion – Israel Institute of Technology</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I61893789</t>
+  </si>
+  <si>
+    <t>TU Bergakademie Freiberg</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I4577782</t>
+  </si>
+  <si>
+    <t>Technical University of Berlin</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I31512782</t>
+  </si>
+  <si>
+    <t>TU Darmstadt</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I78650965</t>
+  </si>
+  <si>
+    <t>TU Dresden</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I153267046</t>
+  </si>
+  <si>
+    <t>University of Kaiserslautern</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I98461037</t>
+  </si>
+  <si>
+    <t>Monterrey Institute of Technology and Higher Education</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I91045830</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I162030827</t>
+  </si>
+  <si>
+    <t>Thapar University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I197251160</t>
+  </si>
+  <si>
+    <t>Hebrew University of Jerusalem</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I98677209</t>
+  </si>
+  <si>
+    <t>University of Edinburgh</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I28407311</t>
+  </si>
+  <si>
+    <t>University of Manchester</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I91136226</t>
+  </si>
+  <si>
+    <t>University of Sheffield</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I74801974</t>
+  </si>
+  <si>
+    <t>University of Tokyo</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I39555362</t>
+  </si>
+  <si>
+    <t>University of Warwick</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I205274468</t>
+  </si>
+  <si>
+    <t>Trinity College Dublin</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I196349391</t>
+  </si>
+  <si>
+    <t>University of Ulm</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I63634437</t>
+  </si>
+  <si>
+    <t>Autonomous University of Madrid</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I52354020</t>
+  </si>
+  <si>
+    <t>University of Almería</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I172787465</t>
+  </si>
+  <si>
+    <t>University of Concepción</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I158438070</t>
+  </si>
+  <si>
+    <t>University of La Laguna</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I180910786</t>
+  </si>
+  <si>
+    <t>University of the Republic</t>
+  </si>
+  <si>
+    <t>UY</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I36243813</t>
+  </si>
+  <si>
+    <t>National University of Colombia</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I874386039</t>
+  </si>
+  <si>
+    <t>National University of La Plata</t>
+  </si>
+  <si>
+    <t>University of Brasília</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I150729083</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I141596103</t>
+  </si>
+  <si>
+    <t>University of Lisbon</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I879563668</t>
+  </si>
+  <si>
+    <t>São Paulo State University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I126158947</t>
+  </si>
+  <si>
+    <t>Federal University of Bahia</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I88273585</t>
+  </si>
+  <si>
+    <t>Federal University of São Paulo</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I52418104</t>
+  </si>
+  <si>
+    <t>Federal University of Paraná</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I122140584</t>
+  </si>
+  <si>
+    <t>Federal University of Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I161127581</t>
+  </si>
+  <si>
+    <t>Fluminense Federal University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I103320735</t>
+  </si>
+  <si>
+    <t>Catholic University of the Sacred Heart</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I142910587</t>
+  </si>
+  <si>
+    <t>University of Salento</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I122534668</t>
+  </si>
+  <si>
+    <t>Marche Polytechnic University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I123044942</t>
+  </si>
+  <si>
+    <t>Autonomous University of Barcelona</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I10902133</t>
+  </si>
+  <si>
+    <t>Jaume I University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I9617848</t>
+  </si>
+  <si>
+    <t>Universitat Politècnica de Catalunya</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I60668342</t>
+  </si>
+  <si>
+    <t>University of Regensburg</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I55952717</t>
+  </si>
+  <si>
+    <t>Rovira i Virgili University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I9341345</t>
+  </si>
+  <si>
+    <t>University of Lübeck</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I90183372</t>
+  </si>
+  <si>
+    <t>University of Lorraine</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I70931966</t>
+  </si>
+  <si>
+    <t>University of Montreal</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I97188460</t>
+  </si>
+  <si>
+    <t>University of Nantes</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I204730241</t>
+  </si>
+  <si>
+    <t>University of Paris</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I110017253</t>
+  </si>
+  <si>
+    <t>François Rabelais University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I63596082</t>
+  </si>
+  <si>
+    <t>Tunis El Manar University</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I195731000</t>
+  </si>
+  <si>
+    <t>Versailles Saint-Quentin-en-Yvelines University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I157169809</t>
+  </si>
+  <si>
+    <t>University of Sciences and Technology Houari Boumediene</t>
+  </si>
+  <si>
+    <t>DZ</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I159129438</t>
+  </si>
+  <si>
+    <t>University of Quebec at Montreal</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I899635006</t>
+  </si>
+  <si>
+    <t>Grenoble Alpes University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I2746051580</t>
+  </si>
+  <si>
+    <t>PSL Research University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I2800365227</t>
+  </si>
+  <si>
+    <t>University of Paris-Est</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I277688954</t>
+  </si>
+  <si>
+    <t>University of Paris-Saclay</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I4210091279</t>
+  </si>
+  <si>
+    <t>Paris 13 University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I134560555</t>
+  </si>
+  <si>
+    <t>Paul Sabatier University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I2801594805</t>
+  </si>
+  <si>
+    <t>University Kebangsaan Malaysia Medical Centre</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I4576418</t>
+  </si>
+  <si>
+    <t>University of Technology Malaysia</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I392282</t>
+  </si>
+  <si>
+    <t>University at Albany, State University of New York</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I63190737</t>
+  </si>
+  <si>
+    <t>University at Buffalo, State University of New York</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I32389192</t>
+  </si>
+  <si>
+    <t>University of Alabama at Birmingham</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I17301866</t>
+  </si>
+  <si>
+    <t>University of Alabama</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I79620101</t>
+  </si>
+  <si>
+    <t>University of Arkansas for Medical Sciences</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I78715868</t>
+  </si>
+  <si>
+    <t>University of Arkansas at Fayetteville</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I98702875</t>
+  </si>
+  <si>
+    <t>Université de Caen Normandie</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I181391015</t>
+  </si>
+  <si>
+    <t>State University of Campinas</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I9073902</t>
+  </si>
+  <si>
+    <t>University of Chemistry and Technology</t>
   </si>
 </sst>
 </file>
@@ -2487,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF803885-FA68-4431-A905-937B1B2D1406}">
   <dimension ref="A1:J213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A212" sqref="A165:A212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4910,19 +5393,22 @@
         <v>245</v>
       </c>
       <c r="D83" t="s">
-        <v>18</v>
+        <v>687</v>
       </c>
       <c r="E83" t="s">
-        <v>18</v>
+        <v>688</v>
       </c>
       <c r="F83" t="s">
         <v>18</v>
       </c>
       <c r="G83" t="s">
-        <v>18</v>
+        <v>651</v>
       </c>
       <c r="H83" t="s">
-        <v>18</v>
+        <v>183</v>
+      </c>
+      <c r="I83" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -4936,19 +5422,22 @@
         <v>247</v>
       </c>
       <c r="D84" t="s">
-        <v>18</v>
+        <v>689</v>
       </c>
       <c r="E84" t="s">
-        <v>18</v>
+        <v>690</v>
       </c>
       <c r="F84" t="s">
         <v>18</v>
       </c>
       <c r="G84" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H84" t="s">
-        <v>18</v>
+        <v>90</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -4962,19 +5451,22 @@
         <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>18</v>
+        <v>691</v>
       </c>
       <c r="E85" t="s">
-        <v>18</v>
+        <v>692</v>
       </c>
       <c r="F85" t="s">
         <v>18</v>
       </c>
       <c r="G85" t="s">
-        <v>18</v>
+        <v>607</v>
       </c>
       <c r="H85" t="s">
-        <v>18</v>
+        <v>122</v>
+      </c>
+      <c r="I85" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -4988,19 +5480,22 @@
         <v>251</v>
       </c>
       <c r="D86" t="s">
-        <v>18</v>
+        <v>693</v>
       </c>
       <c r="E86" t="s">
-        <v>18</v>
+        <v>694</v>
       </c>
       <c r="F86" t="s">
         <v>18</v>
       </c>
       <c r="G86" t="s">
-        <v>18</v>
+        <v>564</v>
       </c>
       <c r="H86" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I86" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -5014,19 +5509,22 @@
         <v>253</v>
       </c>
       <c r="D87" t="s">
-        <v>18</v>
+        <v>695</v>
       </c>
       <c r="E87" t="s">
-        <v>18</v>
+        <v>696</v>
       </c>
       <c r="F87" t="s">
         <v>18</v>
       </c>
       <c r="G87" t="s">
-        <v>18</v>
+        <v>551</v>
       </c>
       <c r="H87" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="I87" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -5040,19 +5538,22 @@
         <v>255</v>
       </c>
       <c r="D88" t="s">
-        <v>18</v>
+        <v>697</v>
       </c>
       <c r="E88" t="s">
-        <v>18</v>
+        <v>698</v>
       </c>
       <c r="F88" t="s">
         <v>18</v>
       </c>
       <c r="G88" t="s">
-        <v>18</v>
+        <v>618</v>
       </c>
       <c r="H88" t="s">
-        <v>18</v>
+        <v>133</v>
+      </c>
+      <c r="I88" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -5066,19 +5567,22 @@
         <v>257</v>
       </c>
       <c r="D89" t="s">
-        <v>18</v>
+        <v>699</v>
       </c>
       <c r="E89" t="s">
-        <v>18</v>
+        <v>700</v>
       </c>
       <c r="F89" t="s">
         <v>18</v>
       </c>
       <c r="G89" t="s">
-        <v>18</v>
+        <v>618</v>
       </c>
       <c r="H89" t="s">
-        <v>18</v>
+        <v>133</v>
+      </c>
+      <c r="I89" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -5106,6 +5610,9 @@
       <c r="H90" t="s">
         <v>52</v>
       </c>
+      <c r="I90" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
@@ -5132,6 +5639,9 @@
       <c r="H91" t="s">
         <v>265</v>
       </c>
+      <c r="I91" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
@@ -5144,19 +5654,22 @@
         <v>267</v>
       </c>
       <c r="D92" t="s">
-        <v>18</v>
+        <v>701</v>
       </c>
       <c r="E92" t="s">
-        <v>18</v>
+        <v>702</v>
       </c>
       <c r="F92" t="s">
         <v>18</v>
       </c>
       <c r="G92" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H92" t="s">
-        <v>18</v>
+        <v>703</v>
+      </c>
+      <c r="I92" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -5170,19 +5683,22 @@
         <v>269</v>
       </c>
       <c r="D93" t="s">
-        <v>18</v>
+        <v>704</v>
       </c>
       <c r="E93" t="s">
-        <v>18</v>
+        <v>705</v>
       </c>
       <c r="F93" t="s">
         <v>18</v>
       </c>
       <c r="G93" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H93" t="s">
-        <v>18</v>
+        <v>703</v>
+      </c>
+      <c r="I93" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -5210,6 +5726,9 @@
       <c r="H94" t="s">
         <v>275</v>
       </c>
+      <c r="I94" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
@@ -5222,19 +5741,22 @@
         <v>278</v>
       </c>
       <c r="D95" t="s">
-        <v>18</v>
+        <v>706</v>
       </c>
       <c r="E95" t="s">
-        <v>18</v>
+        <v>707</v>
       </c>
       <c r="F95" t="s">
         <v>18</v>
       </c>
       <c r="G95" t="s">
-        <v>18</v>
+        <v>708</v>
       </c>
       <c r="H95" t="s">
-        <v>18</v>
+        <v>277</v>
+      </c>
+      <c r="I95" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -5248,22 +5770,25 @@
         <v>280</v>
       </c>
       <c r="D96" t="s">
-        <v>18</v>
+        <v>709</v>
       </c>
       <c r="E96" t="s">
-        <v>18</v>
+        <v>710</v>
       </c>
       <c r="F96" t="s">
         <v>18</v>
       </c>
       <c r="G96" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>281</v>
       </c>
@@ -5274,22 +5799,25 @@
         <v>282</v>
       </c>
       <c r="D97" t="s">
-        <v>18</v>
+        <v>711</v>
       </c>
       <c r="E97" t="s">
-        <v>18</v>
+        <v>712</v>
       </c>
       <c r="F97" t="s">
         <v>18</v>
       </c>
       <c r="G97" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H97" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>283</v>
       </c>
@@ -5300,22 +5828,25 @@
         <v>284</v>
       </c>
       <c r="D98" t="s">
-        <v>18</v>
+        <v>713</v>
       </c>
       <c r="E98" t="s">
-        <v>18</v>
+        <v>714</v>
       </c>
       <c r="F98" t="s">
         <v>18</v>
       </c>
       <c r="G98" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H98" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>285</v>
       </c>
@@ -5326,22 +5857,25 @@
         <v>286</v>
       </c>
       <c r="D99" t="s">
-        <v>18</v>
+        <v>715</v>
       </c>
       <c r="E99" t="s">
-        <v>18</v>
+        <v>716</v>
       </c>
       <c r="F99" t="s">
         <v>18</v>
       </c>
       <c r="G99" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H99" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>287</v>
       </c>
@@ -5352,22 +5886,25 @@
         <v>288</v>
       </c>
       <c r="D100" t="s">
-        <v>18</v>
+        <v>717</v>
       </c>
       <c r="E100" t="s">
-        <v>18</v>
+        <v>718</v>
       </c>
       <c r="F100" t="s">
         <v>18</v>
       </c>
       <c r="G100" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H100" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>289</v>
       </c>
@@ -5378,22 +5915,25 @@
         <v>290</v>
       </c>
       <c r="D101" t="s">
-        <v>18</v>
+        <v>719</v>
       </c>
       <c r="E101" t="s">
-        <v>18</v>
+        <v>720</v>
       </c>
       <c r="F101" t="s">
         <v>18</v>
       </c>
       <c r="G101" t="s">
-        <v>18</v>
+        <v>559</v>
       </c>
       <c r="H101" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="I101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>291</v>
       </c>
@@ -5404,22 +5944,25 @@
         <v>292</v>
       </c>
       <c r="D102" t="s">
-        <v>18</v>
+        <v>721</v>
       </c>
       <c r="E102" t="s">
-        <v>18</v>
+        <v>722</v>
       </c>
       <c r="F102" t="s">
         <v>18</v>
       </c>
       <c r="G102" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H102" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>293</v>
       </c>
@@ -5430,22 +5973,25 @@
         <v>294</v>
       </c>
       <c r="D103" t="s">
-        <v>18</v>
+        <v>723</v>
       </c>
       <c r="E103" t="s">
-        <v>18</v>
+        <v>724</v>
       </c>
       <c r="F103" t="s">
         <v>18</v>
       </c>
       <c r="G103" t="s">
-        <v>18</v>
+        <v>551</v>
       </c>
       <c r="H103" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>295</v>
       </c>
@@ -5456,22 +6002,25 @@
         <v>296</v>
       </c>
       <c r="D104" t="s">
-        <v>18</v>
+        <v>725</v>
       </c>
       <c r="E104" t="s">
-        <v>18</v>
+        <v>726</v>
       </c>
       <c r="F104" t="s">
         <v>18</v>
       </c>
       <c r="G104" t="s">
-        <v>18</v>
+        <v>708</v>
       </c>
       <c r="H104" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+      <c r="I104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>297</v>
       </c>
@@ -5482,22 +6031,25 @@
         <v>298</v>
       </c>
       <c r="D105" t="s">
-        <v>18</v>
+        <v>727</v>
       </c>
       <c r="E105" t="s">
-        <v>18</v>
+        <v>728</v>
       </c>
       <c r="F105" t="s">
         <v>18</v>
       </c>
       <c r="G105" t="s">
-        <v>18</v>
+        <v>568</v>
       </c>
       <c r="H105" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>299</v>
       </c>
@@ -5508,22 +6060,25 @@
         <v>300</v>
       </c>
       <c r="D106" t="s">
-        <v>18</v>
+        <v>729</v>
       </c>
       <c r="E106" t="s">
-        <v>18</v>
+        <v>730</v>
       </c>
       <c r="F106" t="s">
         <v>18</v>
       </c>
       <c r="G106" t="s">
-        <v>18</v>
+        <v>568</v>
       </c>
       <c r="H106" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>301</v>
       </c>
@@ -5534,22 +6089,25 @@
         <v>302</v>
       </c>
       <c r="D107" t="s">
-        <v>18</v>
+        <v>731</v>
       </c>
       <c r="E107" t="s">
-        <v>18</v>
+        <v>732</v>
       </c>
       <c r="F107" t="s">
         <v>18</v>
       </c>
       <c r="G107" t="s">
-        <v>18</v>
+        <v>568</v>
       </c>
       <c r="H107" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>303</v>
       </c>
@@ -5560,22 +6118,25 @@
         <v>304</v>
       </c>
       <c r="D108" t="s">
-        <v>18</v>
+        <v>733</v>
       </c>
       <c r="E108" t="s">
-        <v>18</v>
+        <v>734</v>
       </c>
       <c r="F108" t="s">
         <v>18</v>
       </c>
       <c r="G108" t="s">
-        <v>18</v>
+        <v>167</v>
       </c>
       <c r="H108" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="I108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>305</v>
       </c>
@@ -5586,22 +6147,25 @@
         <v>306</v>
       </c>
       <c r="D109" t="s">
-        <v>18</v>
+        <v>735</v>
       </c>
       <c r="E109" t="s">
-        <v>18</v>
+        <v>736</v>
       </c>
       <c r="F109" t="s">
         <v>18</v>
       </c>
       <c r="G109" t="s">
-        <v>18</v>
+        <v>568</v>
       </c>
       <c r="H109" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>307</v>
       </c>
@@ -5626,8 +6190,11 @@
       <c r="H110" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>314</v>
       </c>
@@ -5638,22 +6205,25 @@
         <v>316</v>
       </c>
       <c r="D111" t="s">
-        <v>18</v>
+        <v>737</v>
       </c>
       <c r="E111" t="s">
-        <v>18</v>
+        <v>738</v>
       </c>
       <c r="F111" t="s">
         <v>18</v>
       </c>
       <c r="G111" t="s">
-        <v>18</v>
+        <v>739</v>
       </c>
       <c r="H111" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="I111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>317</v>
       </c>
@@ -5664,22 +6234,25 @@
         <v>318</v>
       </c>
       <c r="D112" t="s">
-        <v>18</v>
+        <v>740</v>
       </c>
       <c r="E112" t="s">
-        <v>18</v>
+        <v>741</v>
       </c>
       <c r="F112" t="s">
         <v>18</v>
       </c>
       <c r="G112" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H112" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>319</v>
       </c>
@@ -5690,22 +6263,25 @@
         <v>320</v>
       </c>
       <c r="D113" t="s">
-        <v>18</v>
+        <v>742</v>
       </c>
       <c r="E113" t="s">
-        <v>18</v>
+        <v>743</v>
       </c>
       <c r="F113" t="s">
         <v>18</v>
       </c>
       <c r="G113" t="s">
-        <v>18</v>
+        <v>651</v>
       </c>
       <c r="H113" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="I113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>321</v>
       </c>
@@ -5716,22 +6292,25 @@
         <v>322</v>
       </c>
       <c r="D114" t="s">
-        <v>18</v>
+        <v>744</v>
       </c>
       <c r="E114" t="s">
-        <v>18</v>
+        <v>745</v>
       </c>
       <c r="F114" t="s">
         <v>18</v>
       </c>
       <c r="G114" t="s">
-        <v>18</v>
+        <v>651</v>
       </c>
       <c r="H114" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="I114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>323</v>
       </c>
@@ -5742,22 +6321,25 @@
         <v>325</v>
       </c>
       <c r="D115" t="s">
-        <v>18</v>
+        <v>746</v>
       </c>
       <c r="E115" t="s">
-        <v>18</v>
+        <v>747</v>
       </c>
       <c r="F115" t="s">
         <v>18</v>
       </c>
       <c r="G115" t="s">
-        <v>18</v>
+        <v>748</v>
       </c>
       <c r="H115" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="I115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>326</v>
       </c>
@@ -5768,22 +6350,25 @@
         <v>327</v>
       </c>
       <c r="D116" t="s">
-        <v>18</v>
+        <v>749</v>
       </c>
       <c r="E116" t="s">
-        <v>18</v>
+        <v>750</v>
       </c>
       <c r="F116" t="s">
         <v>18</v>
       </c>
       <c r="G116" t="s">
-        <v>18</v>
+        <v>651</v>
       </c>
       <c r="H116" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="I116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>328</v>
       </c>
@@ -5794,22 +6379,25 @@
         <v>330</v>
       </c>
       <c r="D117" t="s">
-        <v>18</v>
+        <v>751</v>
       </c>
       <c r="E117" t="s">
-        <v>18</v>
+        <v>752</v>
       </c>
       <c r="F117" t="s">
         <v>18</v>
       </c>
       <c r="G117" t="s">
-        <v>18</v>
+        <v>753</v>
       </c>
       <c r="H117" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="I117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>331</v>
       </c>
@@ -5834,8 +6422,11 @@
       <c r="H118" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>338</v>
       </c>
@@ -5846,22 +6437,25 @@
         <v>339</v>
       </c>
       <c r="D119" t="s">
-        <v>18</v>
+        <v>754</v>
       </c>
       <c r="E119" t="s">
-        <v>18</v>
+        <v>755</v>
       </c>
       <c r="F119" t="s">
         <v>18</v>
       </c>
       <c r="G119" t="s">
-        <v>18</v>
+        <v>437</v>
       </c>
       <c r="H119" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+      <c r="I119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>340</v>
       </c>
@@ -5872,22 +6466,25 @@
         <v>342</v>
       </c>
       <c r="D120" t="s">
-        <v>18</v>
+        <v>756</v>
       </c>
       <c r="E120" t="s">
-        <v>18</v>
+        <v>757</v>
       </c>
       <c r="F120" t="s">
         <v>18</v>
       </c>
       <c r="G120" t="s">
-        <v>18</v>
+        <v>483</v>
       </c>
       <c r="H120" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+      <c r="I120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>343</v>
       </c>
@@ -5898,22 +6495,25 @@
         <v>344</v>
       </c>
       <c r="D121" t="s">
-        <v>18</v>
+        <v>759</v>
       </c>
       <c r="E121" t="s">
-        <v>18</v>
+        <v>758</v>
       </c>
       <c r="F121" t="s">
         <v>18</v>
       </c>
       <c r="G121" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H121" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>345</v>
       </c>
@@ -5924,22 +6524,25 @@
         <v>347</v>
       </c>
       <c r="D122" t="s">
-        <v>18</v>
+        <v>760</v>
       </c>
       <c r="E122" t="s">
-        <v>18</v>
+        <v>761</v>
       </c>
       <c r="F122" t="s">
         <v>18</v>
       </c>
       <c r="G122" t="s">
-        <v>18</v>
+        <v>762</v>
       </c>
       <c r="H122" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+      <c r="I122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>348</v>
       </c>
@@ -5950,22 +6553,25 @@
         <v>349</v>
       </c>
       <c r="D123" t="s">
-        <v>18</v>
+        <v>763</v>
       </c>
       <c r="E123" t="s">
-        <v>18</v>
+        <v>764</v>
       </c>
       <c r="F123" t="s">
         <v>18</v>
       </c>
       <c r="G123" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H123" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>350</v>
       </c>
@@ -5976,22 +6582,25 @@
         <v>351</v>
       </c>
       <c r="D124" t="s">
-        <v>18</v>
+        <v>765</v>
       </c>
       <c r="E124" t="s">
-        <v>18</v>
+        <v>766</v>
       </c>
       <c r="F124" t="s">
         <v>18</v>
       </c>
       <c r="G124" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H124" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>352</v>
       </c>
@@ -6002,22 +6611,25 @@
         <v>353</v>
       </c>
       <c r="D125" t="s">
-        <v>18</v>
+        <v>767</v>
       </c>
       <c r="E125" t="s">
-        <v>18</v>
+        <v>768</v>
       </c>
       <c r="F125" t="s">
         <v>18</v>
       </c>
       <c r="G125" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H125" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>354</v>
       </c>
@@ -6028,22 +6640,25 @@
         <v>355</v>
       </c>
       <c r="D126" t="s">
-        <v>18</v>
+        <v>769</v>
       </c>
       <c r="E126" t="s">
-        <v>18</v>
+        <v>770</v>
       </c>
       <c r="F126" t="s">
         <v>18</v>
       </c>
       <c r="G126" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H126" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>356</v>
       </c>
@@ -6054,22 +6669,25 @@
         <v>357</v>
       </c>
       <c r="D127" t="s">
-        <v>18</v>
+        <v>771</v>
       </c>
       <c r="E127" t="s">
-        <v>18</v>
+        <v>772</v>
       </c>
       <c r="F127" t="s">
         <v>18</v>
       </c>
       <c r="G127" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H127" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>358</v>
       </c>
@@ -6080,22 +6698,25 @@
         <v>359</v>
       </c>
       <c r="D128" t="s">
-        <v>18</v>
+        <v>773</v>
       </c>
       <c r="E128" t="s">
-        <v>18</v>
+        <v>774</v>
       </c>
       <c r="F128" t="s">
         <v>18</v>
       </c>
       <c r="G128" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H128" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>360</v>
       </c>
@@ -6106,22 +6727,25 @@
         <v>361</v>
       </c>
       <c r="D129" t="s">
-        <v>18</v>
+        <v>775</v>
       </c>
       <c r="E129" t="s">
-        <v>18</v>
+        <v>776</v>
       </c>
       <c r="F129" t="s">
         <v>18</v>
       </c>
       <c r="G129" t="s">
-        <v>18</v>
+        <v>598</v>
       </c>
       <c r="H129" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="I129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>362</v>
       </c>
@@ -6132,22 +6756,25 @@
         <v>363</v>
       </c>
       <c r="D130" t="s">
-        <v>18</v>
+        <v>777</v>
       </c>
       <c r="E130" t="s">
-        <v>18</v>
+        <v>778</v>
       </c>
       <c r="F130" t="s">
         <v>18</v>
       </c>
       <c r="G130" t="s">
-        <v>18</v>
+        <v>598</v>
       </c>
       <c r="H130" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="I130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>364</v>
       </c>
@@ -6158,22 +6785,25 @@
         <v>365</v>
       </c>
       <c r="D131" t="s">
-        <v>18</v>
+        <v>779</v>
       </c>
       <c r="E131" t="s">
-        <v>18</v>
+        <v>780</v>
       </c>
       <c r="F131" t="s">
         <v>18</v>
       </c>
       <c r="G131" t="s">
-        <v>18</v>
+        <v>598</v>
       </c>
       <c r="H131" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="I131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>366</v>
       </c>
@@ -6184,22 +6814,25 @@
         <v>367</v>
       </c>
       <c r="D132" t="s">
-        <v>18</v>
+        <v>781</v>
       </c>
       <c r="E132" t="s">
-        <v>18</v>
+        <v>782</v>
       </c>
       <c r="F132" t="s">
         <v>18</v>
       </c>
       <c r="G132" t="s">
-        <v>18</v>
+        <v>651</v>
       </c>
       <c r="H132" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="I132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>368</v>
       </c>
@@ -6210,22 +6843,25 @@
         <v>369</v>
       </c>
       <c r="D133" t="s">
-        <v>18</v>
+        <v>783</v>
       </c>
       <c r="E133" t="s">
-        <v>18</v>
+        <v>784</v>
       </c>
       <c r="F133" t="s">
         <v>18</v>
       </c>
       <c r="G133" t="s">
-        <v>18</v>
+        <v>651</v>
       </c>
       <c r="H133" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="I133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>370</v>
       </c>
@@ -6236,22 +6872,25 @@
         <v>371</v>
       </c>
       <c r="D134" t="s">
-        <v>18</v>
+        <v>785</v>
       </c>
       <c r="E134" t="s">
-        <v>18</v>
+        <v>786</v>
       </c>
       <c r="F134" t="s">
         <v>18</v>
       </c>
       <c r="G134" t="s">
-        <v>18</v>
+        <v>651</v>
       </c>
       <c r="H134" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="I134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>372</v>
       </c>
@@ -6262,22 +6901,25 @@
         <v>373</v>
       </c>
       <c r="D135" t="s">
-        <v>18</v>
+        <v>787</v>
       </c>
       <c r="E135" t="s">
-        <v>18</v>
+        <v>788</v>
       </c>
       <c r="F135" t="s">
         <v>18</v>
       </c>
       <c r="G135" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H135" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>374</v>
       </c>
@@ -6288,22 +6930,25 @@
         <v>375</v>
       </c>
       <c r="D136" t="s">
-        <v>18</v>
+        <v>789</v>
       </c>
       <c r="E136" t="s">
-        <v>18</v>
+        <v>790</v>
       </c>
       <c r="F136" t="s">
         <v>18</v>
       </c>
       <c r="G136" t="s">
-        <v>18</v>
+        <v>651</v>
       </c>
       <c r="H136" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="I136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>376</v>
       </c>
@@ -6314,22 +6959,25 @@
         <v>377</v>
       </c>
       <c r="D137" t="s">
-        <v>18</v>
+        <v>791</v>
       </c>
       <c r="E137" t="s">
-        <v>18</v>
+        <v>792</v>
       </c>
       <c r="F137" t="s">
         <v>18</v>
       </c>
       <c r="G137" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
       <c r="H137" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>378</v>
       </c>
@@ -6340,22 +6988,25 @@
         <v>379</v>
       </c>
       <c r="D138" t="s">
-        <v>18</v>
+        <v>793</v>
       </c>
       <c r="E138" t="s">
-        <v>18</v>
+        <v>794</v>
       </c>
       <c r="F138" t="s">
         <v>18</v>
       </c>
       <c r="G138" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H138" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>380</v>
       </c>
@@ -6366,22 +7017,25 @@
         <v>381</v>
       </c>
       <c r="D139" t="s">
-        <v>18</v>
+        <v>795</v>
       </c>
       <c r="E139" t="s">
-        <v>18</v>
+        <v>796</v>
       </c>
       <c r="F139" t="s">
         <v>18</v>
       </c>
       <c r="G139" t="s">
-        <v>18</v>
+        <v>797</v>
       </c>
       <c r="H139" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="I139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>382</v>
       </c>
@@ -6392,22 +7046,25 @@
         <v>383</v>
       </c>
       <c r="D140" t="s">
-        <v>18</v>
+        <v>798</v>
       </c>
       <c r="E140" t="s">
-        <v>18</v>
+        <v>799</v>
       </c>
       <c r="F140" t="s">
         <v>18</v>
       </c>
       <c r="G140" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H140" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>384</v>
       </c>
@@ -6418,22 +7075,25 @@
         <v>385</v>
       </c>
       <c r="D141" t="s">
-        <v>18</v>
+        <v>800</v>
       </c>
       <c r="E141" t="s">
-        <v>18</v>
+        <v>801</v>
       </c>
       <c r="F141" t="s">
         <v>18</v>
       </c>
       <c r="G141" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H141" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>386</v>
       </c>
@@ -6444,22 +7104,25 @@
         <v>387</v>
       </c>
       <c r="D142" t="s">
-        <v>18</v>
+        <v>802</v>
       </c>
       <c r="E142" t="s">
-        <v>18</v>
+        <v>803</v>
       </c>
       <c r="F142" t="s">
         <v>18</v>
       </c>
       <c r="G142" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H142" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>388</v>
       </c>
@@ -6470,22 +7133,25 @@
         <v>390</v>
       </c>
       <c r="D143" t="s">
-        <v>18</v>
+        <v>804</v>
       </c>
       <c r="E143" t="s">
-        <v>18</v>
+        <v>805</v>
       </c>
       <c r="F143" t="s">
         <v>18</v>
       </c>
       <c r="G143" t="s">
-        <v>18</v>
+        <v>806</v>
       </c>
       <c r="H143" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+      <c r="I143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>391</v>
       </c>
@@ -6496,22 +7162,25 @@
         <v>392</v>
       </c>
       <c r="D144" t="s">
-        <v>18</v>
+        <v>807</v>
       </c>
       <c r="E144" t="s">
-        <v>18</v>
+        <v>808</v>
       </c>
       <c r="F144" t="s">
         <v>18</v>
       </c>
       <c r="G144" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H144" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>393</v>
       </c>
@@ -6522,22 +7191,25 @@
         <v>395</v>
       </c>
       <c r="D145" t="s">
-        <v>18</v>
+        <v>809</v>
       </c>
       <c r="E145" t="s">
-        <v>18</v>
+        <v>810</v>
       </c>
       <c r="F145" t="s">
         <v>18</v>
       </c>
       <c r="G145" t="s">
-        <v>18</v>
+        <v>811</v>
       </c>
       <c r="H145" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+      <c r="I145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>396</v>
       </c>
@@ -6548,22 +7220,25 @@
         <v>397</v>
       </c>
       <c r="D146" t="s">
-        <v>18</v>
+        <v>812</v>
       </c>
       <c r="E146" t="s">
-        <v>18</v>
+        <v>813</v>
       </c>
       <c r="F146" t="s">
         <v>18</v>
       </c>
       <c r="G146" t="s">
-        <v>18</v>
+        <v>797</v>
       </c>
       <c r="H146" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="I146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>398</v>
       </c>
@@ -6574,22 +7249,25 @@
         <v>399</v>
       </c>
       <c r="D147" t="s">
-        <v>18</v>
+        <v>814</v>
       </c>
       <c r="E147" t="s">
-        <v>18</v>
+        <v>815</v>
       </c>
       <c r="F147" t="s">
         <v>18</v>
       </c>
       <c r="G147" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H147" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>400</v>
       </c>
@@ -6600,22 +7278,25 @@
         <v>401</v>
       </c>
       <c r="D148" t="s">
-        <v>18</v>
+        <v>816</v>
       </c>
       <c r="E148" t="s">
-        <v>18</v>
+        <v>817</v>
       </c>
       <c r="F148" t="s">
         <v>18</v>
       </c>
       <c r="G148" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H148" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>402</v>
       </c>
@@ -6626,22 +7307,25 @@
         <v>403</v>
       </c>
       <c r="D149" t="s">
-        <v>18</v>
+        <v>818</v>
       </c>
       <c r="E149" t="s">
-        <v>18</v>
+        <v>819</v>
       </c>
       <c r="F149" t="s">
         <v>18</v>
       </c>
       <c r="G149" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H149" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>404</v>
       </c>
@@ -6652,22 +7336,25 @@
         <v>405</v>
       </c>
       <c r="D150" t="s">
-        <v>18</v>
+        <v>820</v>
       </c>
       <c r="E150" t="s">
-        <v>18</v>
+        <v>821</v>
       </c>
       <c r="F150" t="s">
         <v>18</v>
       </c>
       <c r="G150" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H150" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>406</v>
       </c>
@@ -6678,22 +7365,25 @@
         <v>407</v>
       </c>
       <c r="D151" t="s">
-        <v>18</v>
+        <v>822</v>
       </c>
       <c r="E151" t="s">
-        <v>18</v>
+        <v>823</v>
       </c>
       <c r="F151" t="s">
         <v>18</v>
       </c>
       <c r="G151" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H151" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>408</v>
       </c>
@@ -6704,22 +7394,25 @@
         <v>409</v>
       </c>
       <c r="D152" t="s">
-        <v>18</v>
+        <v>824</v>
       </c>
       <c r="E152" t="s">
-        <v>18</v>
+        <v>825</v>
       </c>
       <c r="F152" t="s">
         <v>18</v>
       </c>
       <c r="G152" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H152" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>410</v>
       </c>
@@ -6730,22 +7423,25 @@
         <v>411</v>
       </c>
       <c r="D153" t="s">
-        <v>18</v>
+        <v>826</v>
       </c>
       <c r="E153" t="s">
-        <v>18</v>
+        <v>827</v>
       </c>
       <c r="F153" t="s">
         <v>18</v>
       </c>
       <c r="G153" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="H153" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="I153" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>412</v>
       </c>
@@ -6756,22 +7452,25 @@
         <v>413</v>
       </c>
       <c r="D154" t="s">
-        <v>18</v>
+        <v>828</v>
       </c>
       <c r="E154" t="s">
-        <v>18</v>
+        <v>829</v>
       </c>
       <c r="F154" t="s">
         <v>18</v>
       </c>
       <c r="G154" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="H154" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="I154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>414</v>
       </c>
@@ -6782,22 +7481,25 @@
         <v>415</v>
       </c>
       <c r="D155" t="s">
-        <v>18</v>
+        <v>830</v>
       </c>
       <c r="E155" t="s">
-        <v>18</v>
+        <v>831</v>
       </c>
       <c r="F155" t="s">
         <v>18</v>
       </c>
       <c r="G155" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H155" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>416</v>
       </c>
@@ -6808,22 +7510,25 @@
         <v>417</v>
       </c>
       <c r="D156" t="s">
-        <v>18</v>
+        <v>832</v>
       </c>
       <c r="E156" t="s">
-        <v>18</v>
+        <v>833</v>
       </c>
       <c r="F156" t="s">
         <v>18</v>
       </c>
       <c r="G156" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H156" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>418</v>
       </c>
@@ -6834,22 +7539,25 @@
         <v>419</v>
       </c>
       <c r="D157" t="s">
-        <v>18</v>
+        <v>834</v>
       </c>
       <c r="E157" t="s">
-        <v>18</v>
+        <v>835</v>
       </c>
       <c r="F157" t="s">
         <v>18</v>
       </c>
       <c r="G157" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H157" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>420</v>
       </c>
@@ -6860,22 +7568,25 @@
         <v>421</v>
       </c>
       <c r="D158" t="s">
-        <v>18</v>
+        <v>836</v>
       </c>
       <c r="E158" t="s">
-        <v>18</v>
+        <v>837</v>
       </c>
       <c r="F158" t="s">
         <v>18</v>
       </c>
       <c r="G158" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H158" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>422</v>
       </c>
@@ -6886,22 +7597,25 @@
         <v>423</v>
       </c>
       <c r="D159" t="s">
-        <v>18</v>
+        <v>838</v>
       </c>
       <c r="E159" t="s">
-        <v>18</v>
+        <v>839</v>
       </c>
       <c r="F159" t="s">
         <v>18</v>
       </c>
       <c r="G159" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H159" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>424</v>
       </c>
@@ -6912,22 +7626,25 @@
         <v>425</v>
       </c>
       <c r="D160" t="s">
-        <v>18</v>
+        <v>840</v>
       </c>
       <c r="E160" t="s">
-        <v>18</v>
+        <v>841</v>
       </c>
       <c r="F160" t="s">
         <v>18</v>
       </c>
       <c r="G160" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H160" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>426</v>
       </c>
@@ -6938,22 +7655,25 @@
         <v>427</v>
       </c>
       <c r="D161" t="s">
-        <v>18</v>
+        <v>842</v>
       </c>
       <c r="E161" t="s">
-        <v>18</v>
+        <v>843</v>
       </c>
       <c r="F161" t="s">
         <v>18</v>
       </c>
       <c r="G161" t="s">
-        <v>18</v>
+        <v>571</v>
       </c>
       <c r="H161" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>428</v>
       </c>
@@ -6964,22 +7684,25 @@
         <v>429</v>
       </c>
       <c r="D162" t="s">
-        <v>18</v>
+        <v>844</v>
       </c>
       <c r="E162" t="s">
-        <v>18</v>
+        <v>845</v>
       </c>
       <c r="F162" t="s">
         <v>18</v>
       </c>
       <c r="G162" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H162" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I162" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>430</v>
       </c>
@@ -6990,22 +7713,25 @@
         <v>431</v>
       </c>
       <c r="D163" t="s">
-        <v>18</v>
+        <v>846</v>
       </c>
       <c r="E163" t="s">
-        <v>18</v>
+        <v>847</v>
       </c>
       <c r="F163" t="s">
         <v>18</v>
       </c>
       <c r="G163" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="H163" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="I163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>432</v>
       </c>
@@ -7030,8 +7756,11 @@
       <c r="H164" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>438</v>
       </c>
@@ -7057,7 +7786,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>440</v>
       </c>
@@ -7083,7 +7812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>442</v>
       </c>
@@ -7109,7 +7838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>444</v>
       </c>
@@ -7135,7 +7864,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>446</v>
       </c>
@@ -7161,7 +7890,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>448</v>
       </c>
@@ -7187,7 +7916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>450</v>
       </c>
@@ -7213,7 +7942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>452</v>
       </c>
@@ -7239,7 +7968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>454</v>
       </c>
@@ -7265,7 +7994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>456</v>
       </c>
@@ -7291,7 +8020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>458</v>
       </c>
@@ -7317,7 +8046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>460</v>
       </c>
@@ -8175,7 +8904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>536</v>
       </c>
@@ -8201,7 +8930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>538</v>
       </c>
@@ -8227,7 +8956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>540</v>
       </c>
@@ -8253,7 +8982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>542</v>
       </c>
@@ -8279,7 +9008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>544</v>
       </c>
@@ -8303,6 +9032,9 @@
       </c>
       <c r="H213" t="s">
         <v>548</v>
+      </c>
+      <c r="I213" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8312,5 +9044,6 @@
     <hyperlink ref="D39" r:id="rId3" xr:uid="{F0BCB511-D579-4B83-9B99-8266AB4450DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish leiden matching and add csv
</commit_message>
<xml_diff>
--- a/data/processed/leiden_matching_table.xlsx
+++ b/data/processed/leiden_matching_table.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tklebel\Documents\Projects\ON-MERRIT\03-Analysis\apc_effect\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C920C544-2CDE-4D19-A79D-0722E00546AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDEEE68B-C20C-412C-A00E-93EE1CA025D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="7646" windowWidth="22149" windowHeight="12103" xr2:uid="{70655950-438C-47E9-B52C-924540BD7C84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{70655950-438C-47E9-B52C-924540BD7C84}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="leiden_matching_table" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="leiden_unmatched" localSheetId="0">Sheet1!$A$1:$H$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">leiden_matching_table!$A$1:$J$213</definedName>
+    <definedName name="leiden_unmatched" localSheetId="0">leiden_matching_table!$A$1:$H$213</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="938">
   <si>
     <t>University</t>
   </si>
@@ -2166,9 +2167,6 @@
     <t>Saint Louis University</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>https://openalex.org/I59553526</t>
   </si>
   <si>
@@ -2599,6 +2597,279 @@
   </si>
   <si>
     <t>University of Chemistry and Technology</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I165733156</t>
+  </si>
+  <si>
+    <t>University of Georgia</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I117965899</t>
+  </si>
+  <si>
+    <t>University of Hawaii at Manoa</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I4210128276</t>
+  </si>
+  <si>
+    <t>Sağlık Bilimleri Üniversitesi</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I39422238</t>
+  </si>
+  <si>
+    <t>University of Illinois at Chicago</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I143397708</t>
+  </si>
+  <si>
+    <t>Innsbruck Medical University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I158552681</t>
+  </si>
+  <si>
+    <t>University of Life Sciences</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I7947594</t>
+  </si>
+  <si>
+    <t>University of Maine</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I27837315</t>
+  </si>
+  <si>
+    <t>University of Michigan–Ann Arbor</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I130238516</t>
+  </si>
+  <si>
+    <t>University of Minnesota</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I76835614</t>
+  </si>
+  <si>
+    <t>University of Missouri</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I75421653</t>
+  </si>
+  <si>
+    <t>University of Missouri–Kansas City</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I92869138</t>
+  </si>
+  <si>
+    <t>University of Natural Resources and Life Sciences</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I114395901</t>
+  </si>
+  <si>
+    <t>University of Nebraska–Lincoln</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I31746571</t>
+  </si>
+  <si>
+    <t>UNSW Sydney</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I78757542</t>
+  </si>
+  <si>
+    <t>University of Newcastle Australia</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I114027177</t>
+  </si>
+  <si>
+    <t>University of North Carolina at Chapel Hill</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I102149020</t>
+  </si>
+  <si>
+    <t>University of North Carolina at Charlotte</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I169335092</t>
+  </si>
+  <si>
+    <t>University of North Carolina at Greensboro</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I138689650</t>
+  </si>
+  <si>
+    <t>University of Padua</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I17974374</t>
+  </si>
+  <si>
+    <t>Universidade de São Paulo</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I864159182</t>
+  </si>
+  <si>
+    <t>University of Silesia</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I155781252</t>
+  </si>
+  <si>
+    <t>University of South Carolina</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I2613432</t>
+  </si>
+  <si>
+    <t>University of South Florida</t>
+  </si>
+  <si>
+    <t>it is unclear to which entitity the leiden ranking refers to: in OpenAlex there are two, since "tampere uni" is a merger of "uni of tampere" and the technical uni.</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I75027704</t>
+  </si>
+  <si>
+    <t>University of Tennessee at Knoxville</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I189196454</t>
+  </si>
+  <si>
+    <t>The University of Texas at Arlington</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I86519309</t>
+  </si>
+  <si>
+    <t>The University of Texas at Austin</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I162577319</t>
+  </si>
+  <si>
+    <t>The University of Texas at Dallas</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I164936912</t>
+  </si>
+  <si>
+    <t>The University of Texas at El Paso</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I45438204</t>
+  </si>
+  <si>
+    <t>The University of Texas at San Antonio</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I919571938</t>
+  </si>
+  <si>
+    <t>The University of Texas Health Science Center at Houston</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I165951966</t>
+  </si>
+  <si>
+    <t>The University of Texas Health Science Center at San Antonio</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I55302922</t>
+  </si>
+  <si>
+    <t>The University of Texas Medical Branch at Galveston</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I867280407</t>
+  </si>
+  <si>
+    <t>The University of Texas Southwestern Medical Center</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I4210165038</t>
+  </si>
+  <si>
+    <t>University of Chinese Academy of Sciences</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I178535277</t>
+  </si>
+  <si>
+    <t>University of the West of England</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I201448701</t>
+  </si>
+  <si>
+    <t>University of Washington</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I135310074</t>
+  </si>
+  <si>
+    <t>University of Wisconsin–Madison</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I43579087</t>
+  </si>
+  <si>
+    <t>University of Wisconsin–Milwaukee</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I876193797</t>
+  </si>
+  <si>
+    <t>Vellore Institute of Technology University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I71270174</t>
+  </si>
+  <si>
+    <t>Victoria University</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I145847075</t>
+  </si>
+  <si>
+    <t>TU Wien</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I859038795</t>
+  </si>
+  <si>
+    <t>Virginia Tech</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I865915315</t>
+  </si>
+  <si>
+    <t>VU Amsterdam</t>
+  </si>
+  <si>
+    <t>https://openalex.org/I155313962</t>
+  </si>
+  <si>
+    <t>West Pomeranian University of Technology</t>
   </si>
 </sst>
 </file>
@@ -2970,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF803885-FA68-4431-A905-937B1B2D1406}">
   <dimension ref="A1:J213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A212" sqref="A165:A212"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4636,10 +4907,10 @@
         <v>179</v>
       </c>
       <c r="D57" t="s">
-        <v>645</v>
+        <v>855</v>
       </c>
       <c r="E57" t="s">
-        <v>646</v>
+        <v>856</v>
       </c>
       <c r="F57" t="s">
         <v>18</v>
@@ -5666,7 +5937,7 @@
         <v>31</v>
       </c>
       <c r="H92" t="s">
-        <v>703</v>
+        <v>25</v>
       </c>
       <c r="I92" t="b">
         <v>1</v>
@@ -5683,10 +5954,10 @@
         <v>269</v>
       </c>
       <c r="D93" t="s">
+        <v>703</v>
+      </c>
+      <c r="E93" t="s">
         <v>704</v>
-      </c>
-      <c r="E93" t="s">
-        <v>705</v>
       </c>
       <c r="F93" t="s">
         <v>18</v>
@@ -5695,7 +5966,7 @@
         <v>31</v>
       </c>
       <c r="H93" t="s">
-        <v>703</v>
+        <v>25</v>
       </c>
       <c r="I93" t="b">
         <v>1</v>
@@ -5741,16 +6012,16 @@
         <v>278</v>
       </c>
       <c r="D95" t="s">
+        <v>705</v>
+      </c>
+      <c r="E95" t="s">
         <v>706</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
+        <v>18</v>
+      </c>
+      <c r="G95" t="s">
         <v>707</v>
-      </c>
-      <c r="F95" t="s">
-        <v>18</v>
-      </c>
-      <c r="G95" t="s">
-        <v>708</v>
       </c>
       <c r="H95" t="s">
         <v>277</v>
@@ -5770,10 +6041,10 @@
         <v>280</v>
       </c>
       <c r="D96" t="s">
+        <v>708</v>
+      </c>
+      <c r="E96" t="s">
         <v>709</v>
-      </c>
-      <c r="E96" t="s">
-        <v>710</v>
       </c>
       <c r="F96" t="s">
         <v>18</v>
@@ -5799,10 +6070,10 @@
         <v>282</v>
       </c>
       <c r="D97" t="s">
+        <v>710</v>
+      </c>
+      <c r="E97" t="s">
         <v>711</v>
-      </c>
-      <c r="E97" t="s">
-        <v>712</v>
       </c>
       <c r="F97" t="s">
         <v>18</v>
@@ -5828,10 +6099,10 @@
         <v>284</v>
       </c>
       <c r="D98" t="s">
+        <v>712</v>
+      </c>
+      <c r="E98" t="s">
         <v>713</v>
-      </c>
-      <c r="E98" t="s">
-        <v>714</v>
       </c>
       <c r="F98" t="s">
         <v>18</v>
@@ -5857,10 +6128,10 @@
         <v>286</v>
       </c>
       <c r="D99" t="s">
+        <v>714</v>
+      </c>
+      <c r="E99" t="s">
         <v>715</v>
-      </c>
-      <c r="E99" t="s">
-        <v>716</v>
       </c>
       <c r="F99" t="s">
         <v>18</v>
@@ -5886,10 +6157,10 @@
         <v>288</v>
       </c>
       <c r="D100" t="s">
+        <v>716</v>
+      </c>
+      <c r="E100" t="s">
         <v>717</v>
-      </c>
-      <c r="E100" t="s">
-        <v>718</v>
       </c>
       <c r="F100" t="s">
         <v>18</v>
@@ -5915,10 +6186,10 @@
         <v>290</v>
       </c>
       <c r="D101" t="s">
+        <v>718</v>
+      </c>
+      <c r="E101" t="s">
         <v>719</v>
-      </c>
-      <c r="E101" t="s">
-        <v>720</v>
       </c>
       <c r="F101" t="s">
         <v>18</v>
@@ -5944,10 +6215,10 @@
         <v>292</v>
       </c>
       <c r="D102" t="s">
+        <v>720</v>
+      </c>
+      <c r="E102" t="s">
         <v>721</v>
-      </c>
-      <c r="E102" t="s">
-        <v>722</v>
       </c>
       <c r="F102" t="s">
         <v>18</v>
@@ -5973,10 +6244,10 @@
         <v>294</v>
       </c>
       <c r="D103" t="s">
+        <v>722</v>
+      </c>
+      <c r="E103" t="s">
         <v>723</v>
-      </c>
-      <c r="E103" t="s">
-        <v>724</v>
       </c>
       <c r="F103" t="s">
         <v>18</v>
@@ -6002,16 +6273,16 @@
         <v>296</v>
       </c>
       <c r="D104" t="s">
+        <v>724</v>
+      </c>
+      <c r="E104" t="s">
         <v>725</v>
       </c>
-      <c r="E104" t="s">
-        <v>726</v>
-      </c>
       <c r="F104" t="s">
         <v>18</v>
       </c>
       <c r="G104" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H104" t="s">
         <v>277</v>
@@ -6031,10 +6302,10 @@
         <v>298</v>
       </c>
       <c r="D105" t="s">
+        <v>726</v>
+      </c>
+      <c r="E105" t="s">
         <v>727</v>
-      </c>
-      <c r="E105" t="s">
-        <v>728</v>
       </c>
       <c r="F105" t="s">
         <v>18</v>
@@ -6060,10 +6331,10 @@
         <v>300</v>
       </c>
       <c r="D106" t="s">
+        <v>728</v>
+      </c>
+      <c r="E106" t="s">
         <v>729</v>
-      </c>
-      <c r="E106" t="s">
-        <v>730</v>
       </c>
       <c r="F106" t="s">
         <v>18</v>
@@ -6089,10 +6360,10 @@
         <v>302</v>
       </c>
       <c r="D107" t="s">
+        <v>730</v>
+      </c>
+      <c r="E107" t="s">
         <v>731</v>
-      </c>
-      <c r="E107" t="s">
-        <v>732</v>
       </c>
       <c r="F107" t="s">
         <v>18</v>
@@ -6118,10 +6389,10 @@
         <v>304</v>
       </c>
       <c r="D108" t="s">
+        <v>732</v>
+      </c>
+      <c r="E108" t="s">
         <v>733</v>
-      </c>
-      <c r="E108" t="s">
-        <v>734</v>
       </c>
       <c r="F108" t="s">
         <v>18</v>
@@ -6147,10 +6418,10 @@
         <v>306</v>
       </c>
       <c r="D109" t="s">
+        <v>734</v>
+      </c>
+      <c r="E109" t="s">
         <v>735</v>
-      </c>
-      <c r="E109" t="s">
-        <v>736</v>
       </c>
       <c r="F109" t="s">
         <v>18</v>
@@ -6205,16 +6476,16 @@
         <v>316</v>
       </c>
       <c r="D111" t="s">
+        <v>736</v>
+      </c>
+      <c r="E111" t="s">
         <v>737</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
+        <v>18</v>
+      </c>
+      <c r="G111" t="s">
         <v>738</v>
-      </c>
-      <c r="F111" t="s">
-        <v>18</v>
-      </c>
-      <c r="G111" t="s">
-        <v>739</v>
       </c>
       <c r="H111" t="s">
         <v>315</v>
@@ -6234,10 +6505,10 @@
         <v>318</v>
       </c>
       <c r="D112" t="s">
+        <v>739</v>
+      </c>
+      <c r="E112" t="s">
         <v>740</v>
-      </c>
-      <c r="E112" t="s">
-        <v>741</v>
       </c>
       <c r="F112" t="s">
         <v>18</v>
@@ -6263,10 +6534,10 @@
         <v>320</v>
       </c>
       <c r="D113" t="s">
+        <v>741</v>
+      </c>
+      <c r="E113" t="s">
         <v>742</v>
-      </c>
-      <c r="E113" t="s">
-        <v>743</v>
       </c>
       <c r="F113" t="s">
         <v>18</v>
@@ -6292,10 +6563,10 @@
         <v>322</v>
       </c>
       <c r="D114" t="s">
+        <v>743</v>
+      </c>
+      <c r="E114" t="s">
         <v>744</v>
-      </c>
-      <c r="E114" t="s">
-        <v>745</v>
       </c>
       <c r="F114" t="s">
         <v>18</v>
@@ -6321,16 +6592,16 @@
         <v>325</v>
       </c>
       <c r="D115" t="s">
+        <v>745</v>
+      </c>
+      <c r="E115" t="s">
         <v>746</v>
       </c>
-      <c r="E115" t="s">
+      <c r="F115" t="s">
+        <v>18</v>
+      </c>
+      <c r="G115" t="s">
         <v>747</v>
-      </c>
-      <c r="F115" t="s">
-        <v>18</v>
-      </c>
-      <c r="G115" t="s">
-        <v>748</v>
       </c>
       <c r="H115" t="s">
         <v>324</v>
@@ -6350,10 +6621,10 @@
         <v>327</v>
       </c>
       <c r="D116" t="s">
+        <v>748</v>
+      </c>
+      <c r="E116" t="s">
         <v>749</v>
-      </c>
-      <c r="E116" t="s">
-        <v>750</v>
       </c>
       <c r="F116" t="s">
         <v>18</v>
@@ -6379,16 +6650,16 @@
         <v>330</v>
       </c>
       <c r="D117" t="s">
+        <v>750</v>
+      </c>
+      <c r="E117" t="s">
         <v>751</v>
       </c>
-      <c r="E117" t="s">
+      <c r="F117" t="s">
+        <v>18</v>
+      </c>
+      <c r="G117" t="s">
         <v>752</v>
-      </c>
-      <c r="F117" t="s">
-        <v>18</v>
-      </c>
-      <c r="G117" t="s">
-        <v>753</v>
       </c>
       <c r="H117" t="s">
         <v>329</v>
@@ -6437,10 +6708,10 @@
         <v>339</v>
       </c>
       <c r="D119" t="s">
+        <v>753</v>
+      </c>
+      <c r="E119" t="s">
         <v>754</v>
-      </c>
-      <c r="E119" t="s">
-        <v>755</v>
       </c>
       <c r="F119" t="s">
         <v>18</v>
@@ -6466,10 +6737,10 @@
         <v>342</v>
       </c>
       <c r="D120" t="s">
+        <v>755</v>
+      </c>
+      <c r="E120" t="s">
         <v>756</v>
-      </c>
-      <c r="E120" t="s">
-        <v>757</v>
       </c>
       <c r="F120" t="s">
         <v>18</v>
@@ -6495,10 +6766,10 @@
         <v>344</v>
       </c>
       <c r="D121" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E121" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F121" t="s">
         <v>18</v>
@@ -6524,16 +6795,16 @@
         <v>347</v>
       </c>
       <c r="D122" t="s">
+        <v>759</v>
+      </c>
+      <c r="E122" t="s">
         <v>760</v>
       </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
+        <v>18</v>
+      </c>
+      <c r="G122" t="s">
         <v>761</v>
-      </c>
-      <c r="F122" t="s">
-        <v>18</v>
-      </c>
-      <c r="G122" t="s">
-        <v>762</v>
       </c>
       <c r="H122" t="s">
         <v>346</v>
@@ -6553,10 +6824,10 @@
         <v>349</v>
       </c>
       <c r="D123" t="s">
+        <v>762</v>
+      </c>
+      <c r="E123" t="s">
         <v>763</v>
-      </c>
-      <c r="E123" t="s">
-        <v>764</v>
       </c>
       <c r="F123" t="s">
         <v>18</v>
@@ -6582,10 +6853,10 @@
         <v>351</v>
       </c>
       <c r="D124" t="s">
+        <v>764</v>
+      </c>
+      <c r="E124" t="s">
         <v>765</v>
-      </c>
-      <c r="E124" t="s">
-        <v>766</v>
       </c>
       <c r="F124" t="s">
         <v>18</v>
@@ -6611,10 +6882,10 @@
         <v>353</v>
       </c>
       <c r="D125" t="s">
+        <v>766</v>
+      </c>
+      <c r="E125" t="s">
         <v>767</v>
-      </c>
-      <c r="E125" t="s">
-        <v>768</v>
       </c>
       <c r="F125" t="s">
         <v>18</v>
@@ -6640,10 +6911,10 @@
         <v>355</v>
       </c>
       <c r="D126" t="s">
+        <v>768</v>
+      </c>
+      <c r="E126" t="s">
         <v>769</v>
-      </c>
-      <c r="E126" t="s">
-        <v>770</v>
       </c>
       <c r="F126" t="s">
         <v>18</v>
@@ -6669,10 +6940,10 @@
         <v>357</v>
       </c>
       <c r="D127" t="s">
+        <v>770</v>
+      </c>
+      <c r="E127" t="s">
         <v>771</v>
-      </c>
-      <c r="E127" t="s">
-        <v>772</v>
       </c>
       <c r="F127" t="s">
         <v>18</v>
@@ -6698,10 +6969,10 @@
         <v>359</v>
       </c>
       <c r="D128" t="s">
+        <v>772</v>
+      </c>
+      <c r="E128" t="s">
         <v>773</v>
-      </c>
-      <c r="E128" t="s">
-        <v>774</v>
       </c>
       <c r="F128" t="s">
         <v>18</v>
@@ -6727,10 +6998,10 @@
         <v>361</v>
       </c>
       <c r="D129" t="s">
+        <v>774</v>
+      </c>
+      <c r="E129" t="s">
         <v>775</v>
-      </c>
-      <c r="E129" t="s">
-        <v>776</v>
       </c>
       <c r="F129" t="s">
         <v>18</v>
@@ -6756,10 +7027,10 @@
         <v>363</v>
       </c>
       <c r="D130" t="s">
+        <v>776</v>
+      </c>
+      <c r="E130" t="s">
         <v>777</v>
-      </c>
-      <c r="E130" t="s">
-        <v>778</v>
       </c>
       <c r="F130" t="s">
         <v>18</v>
@@ -6785,10 +7056,10 @@
         <v>365</v>
       </c>
       <c r="D131" t="s">
+        <v>778</v>
+      </c>
+      <c r="E131" t="s">
         <v>779</v>
-      </c>
-      <c r="E131" t="s">
-        <v>780</v>
       </c>
       <c r="F131" t="s">
         <v>18</v>
@@ -6814,10 +7085,10 @@
         <v>367</v>
       </c>
       <c r="D132" t="s">
+        <v>780</v>
+      </c>
+      <c r="E132" t="s">
         <v>781</v>
-      </c>
-      <c r="E132" t="s">
-        <v>782</v>
       </c>
       <c r="F132" t="s">
         <v>18</v>
@@ -6843,10 +7114,10 @@
         <v>369</v>
       </c>
       <c r="D133" t="s">
+        <v>782</v>
+      </c>
+      <c r="E133" t="s">
         <v>783</v>
-      </c>
-      <c r="E133" t="s">
-        <v>784</v>
       </c>
       <c r="F133" t="s">
         <v>18</v>
@@ -6872,10 +7143,10 @@
         <v>371</v>
       </c>
       <c r="D134" t="s">
+        <v>784</v>
+      </c>
+      <c r="E134" t="s">
         <v>785</v>
-      </c>
-      <c r="E134" t="s">
-        <v>786</v>
       </c>
       <c r="F134" t="s">
         <v>18</v>
@@ -6901,10 +7172,10 @@
         <v>373</v>
       </c>
       <c r="D135" t="s">
+        <v>786</v>
+      </c>
+      <c r="E135" t="s">
         <v>787</v>
-      </c>
-      <c r="E135" t="s">
-        <v>788</v>
       </c>
       <c r="F135" t="s">
         <v>18</v>
@@ -6930,10 +7201,10 @@
         <v>375</v>
       </c>
       <c r="D136" t="s">
+        <v>788</v>
+      </c>
+      <c r="E136" t="s">
         <v>789</v>
-      </c>
-      <c r="E136" t="s">
-        <v>790</v>
       </c>
       <c r="F136" t="s">
         <v>18</v>
@@ -6959,10 +7230,10 @@
         <v>377</v>
       </c>
       <c r="D137" t="s">
+        <v>790</v>
+      </c>
+      <c r="E137" t="s">
         <v>791</v>
-      </c>
-      <c r="E137" t="s">
-        <v>792</v>
       </c>
       <c r="F137" t="s">
         <v>18</v>
@@ -6988,10 +7259,10 @@
         <v>379</v>
       </c>
       <c r="D138" t="s">
+        <v>792</v>
+      </c>
+      <c r="E138" t="s">
         <v>793</v>
-      </c>
-      <c r="E138" t="s">
-        <v>794</v>
       </c>
       <c r="F138" t="s">
         <v>18</v>
@@ -7017,16 +7288,16 @@
         <v>381</v>
       </c>
       <c r="D139" t="s">
+        <v>794</v>
+      </c>
+      <c r="E139" t="s">
         <v>795</v>
       </c>
-      <c r="E139" t="s">
+      <c r="F139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G139" t="s">
         <v>796</v>
-      </c>
-      <c r="F139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G139" t="s">
-        <v>797</v>
       </c>
       <c r="H139" t="s">
         <v>75</v>
@@ -7046,10 +7317,10 @@
         <v>383</v>
       </c>
       <c r="D140" t="s">
+        <v>797</v>
+      </c>
+      <c r="E140" t="s">
         <v>798</v>
-      </c>
-      <c r="E140" t="s">
-        <v>799</v>
       </c>
       <c r="F140" t="s">
         <v>18</v>
@@ -7075,10 +7346,10 @@
         <v>385</v>
       </c>
       <c r="D141" t="s">
+        <v>799</v>
+      </c>
+      <c r="E141" t="s">
         <v>800</v>
-      </c>
-      <c r="E141" t="s">
-        <v>801</v>
       </c>
       <c r="F141" t="s">
         <v>18</v>
@@ -7104,10 +7375,10 @@
         <v>387</v>
       </c>
       <c r="D142" t="s">
+        <v>801</v>
+      </c>
+      <c r="E142" t="s">
         <v>802</v>
-      </c>
-      <c r="E142" t="s">
-        <v>803</v>
       </c>
       <c r="F142" t="s">
         <v>18</v>
@@ -7133,16 +7404,16 @@
         <v>390</v>
       </c>
       <c r="D143" t="s">
+        <v>803</v>
+      </c>
+      <c r="E143" t="s">
         <v>804</v>
       </c>
-      <c r="E143" t="s">
+      <c r="F143" t="s">
+        <v>18</v>
+      </c>
+      <c r="G143" t="s">
         <v>805</v>
-      </c>
-      <c r="F143" t="s">
-        <v>18</v>
-      </c>
-      <c r="G143" t="s">
-        <v>806</v>
       </c>
       <c r="H143" t="s">
         <v>389</v>
@@ -7162,10 +7433,10 @@
         <v>392</v>
       </c>
       <c r="D144" t="s">
+        <v>806</v>
+      </c>
+      <c r="E144" t="s">
         <v>807</v>
-      </c>
-      <c r="E144" t="s">
-        <v>808</v>
       </c>
       <c r="F144" t="s">
         <v>18</v>
@@ -7191,16 +7462,16 @@
         <v>395</v>
       </c>
       <c r="D145" t="s">
+        <v>808</v>
+      </c>
+      <c r="E145" t="s">
         <v>809</v>
       </c>
-      <c r="E145" t="s">
+      <c r="F145" t="s">
+        <v>18</v>
+      </c>
+      <c r="G145" t="s">
         <v>810</v>
-      </c>
-      <c r="F145" t="s">
-        <v>18</v>
-      </c>
-      <c r="G145" t="s">
-        <v>811</v>
       </c>
       <c r="H145" t="s">
         <v>394</v>
@@ -7220,16 +7491,16 @@
         <v>397</v>
       </c>
       <c r="D146" t="s">
+        <v>811</v>
+      </c>
+      <c r="E146" t="s">
         <v>812</v>
       </c>
-      <c r="E146" t="s">
-        <v>813</v>
-      </c>
       <c r="F146" t="s">
         <v>18</v>
       </c>
       <c r="G146" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H146" t="s">
         <v>75</v>
@@ -7249,10 +7520,10 @@
         <v>399</v>
       </c>
       <c r="D147" t="s">
+        <v>813</v>
+      </c>
+      <c r="E147" t="s">
         <v>814</v>
-      </c>
-      <c r="E147" t="s">
-        <v>815</v>
       </c>
       <c r="F147" t="s">
         <v>18</v>
@@ -7278,10 +7549,10 @@
         <v>401</v>
       </c>
       <c r="D148" t="s">
+        <v>815</v>
+      </c>
+      <c r="E148" t="s">
         <v>816</v>
-      </c>
-      <c r="E148" t="s">
-        <v>817</v>
       </c>
       <c r="F148" t="s">
         <v>18</v>
@@ -7307,10 +7578,10 @@
         <v>403</v>
       </c>
       <c r="D149" t="s">
+        <v>817</v>
+      </c>
+      <c r="E149" t="s">
         <v>818</v>
-      </c>
-      <c r="E149" t="s">
-        <v>819</v>
       </c>
       <c r="F149" t="s">
         <v>18</v>
@@ -7336,10 +7607,10 @@
         <v>405</v>
       </c>
       <c r="D150" t="s">
+        <v>819</v>
+      </c>
+      <c r="E150" t="s">
         <v>820</v>
-      </c>
-      <c r="E150" t="s">
-        <v>821</v>
       </c>
       <c r="F150" t="s">
         <v>18</v>
@@ -7365,10 +7636,10 @@
         <v>407</v>
       </c>
       <c r="D151" t="s">
+        <v>821</v>
+      </c>
+      <c r="E151" t="s">
         <v>822</v>
-      </c>
-      <c r="E151" t="s">
-        <v>823</v>
       </c>
       <c r="F151" t="s">
         <v>18</v>
@@ -7394,10 +7665,10 @@
         <v>409</v>
       </c>
       <c r="D152" t="s">
+        <v>823</v>
+      </c>
+      <c r="E152" t="s">
         <v>824</v>
-      </c>
-      <c r="E152" t="s">
-        <v>825</v>
       </c>
       <c r="F152" t="s">
         <v>18</v>
@@ -7423,10 +7694,10 @@
         <v>411</v>
       </c>
       <c r="D153" t="s">
+        <v>825</v>
+      </c>
+      <c r="E153" t="s">
         <v>826</v>
-      </c>
-      <c r="E153" t="s">
-        <v>827</v>
       </c>
       <c r="F153" t="s">
         <v>18</v>
@@ -7452,10 +7723,10 @@
         <v>413</v>
       </c>
       <c r="D154" t="s">
+        <v>827</v>
+      </c>
+      <c r="E154" t="s">
         <v>828</v>
-      </c>
-      <c r="E154" t="s">
-        <v>829</v>
       </c>
       <c r="F154" t="s">
         <v>18</v>
@@ -7481,10 +7752,10 @@
         <v>415</v>
       </c>
       <c r="D155" t="s">
+        <v>829</v>
+      </c>
+      <c r="E155" t="s">
         <v>830</v>
-      </c>
-      <c r="E155" t="s">
-        <v>831</v>
       </c>
       <c r="F155" t="s">
         <v>18</v>
@@ -7510,10 +7781,10 @@
         <v>417</v>
       </c>
       <c r="D156" t="s">
+        <v>831</v>
+      </c>
+      <c r="E156" t="s">
         <v>832</v>
-      </c>
-      <c r="E156" t="s">
-        <v>833</v>
       </c>
       <c r="F156" t="s">
         <v>18</v>
@@ -7539,10 +7810,10 @@
         <v>419</v>
       </c>
       <c r="D157" t="s">
+        <v>833</v>
+      </c>
+      <c r="E157" t="s">
         <v>834</v>
-      </c>
-      <c r="E157" t="s">
-        <v>835</v>
       </c>
       <c r="F157" t="s">
         <v>18</v>
@@ -7568,10 +7839,10 @@
         <v>421</v>
       </c>
       <c r="D158" t="s">
+        <v>835</v>
+      </c>
+      <c r="E158" t="s">
         <v>836</v>
-      </c>
-      <c r="E158" t="s">
-        <v>837</v>
       </c>
       <c r="F158" t="s">
         <v>18</v>
@@ -7597,10 +7868,10 @@
         <v>423</v>
       </c>
       <c r="D159" t="s">
+        <v>837</v>
+      </c>
+      <c r="E159" t="s">
         <v>838</v>
-      </c>
-      <c r="E159" t="s">
-        <v>839</v>
       </c>
       <c r="F159" t="s">
         <v>18</v>
@@ -7626,10 +7897,10 @@
         <v>425</v>
       </c>
       <c r="D160" t="s">
+        <v>839</v>
+      </c>
+      <c r="E160" t="s">
         <v>840</v>
-      </c>
-      <c r="E160" t="s">
-        <v>841</v>
       </c>
       <c r="F160" t="s">
         <v>18</v>
@@ -7655,10 +7926,10 @@
         <v>427</v>
       </c>
       <c r="D161" t="s">
+        <v>841</v>
+      </c>
+      <c r="E161" t="s">
         <v>842</v>
-      </c>
-      <c r="E161" t="s">
-        <v>843</v>
       </c>
       <c r="F161" t="s">
         <v>18</v>
@@ -7684,10 +7955,10 @@
         <v>429</v>
       </c>
       <c r="D162" t="s">
+        <v>843</v>
+      </c>
+      <c r="E162" t="s">
         <v>844</v>
-      </c>
-      <c r="E162" t="s">
-        <v>845</v>
       </c>
       <c r="F162" t="s">
         <v>18</v>
@@ -7713,10 +7984,10 @@
         <v>431</v>
       </c>
       <c r="D163" t="s">
+        <v>845</v>
+      </c>
+      <c r="E163" t="s">
         <v>846</v>
-      </c>
-      <c r="E163" t="s">
-        <v>847</v>
       </c>
       <c r="F163" t="s">
         <v>18</v>
@@ -7771,19 +8042,22 @@
         <v>439</v>
       </c>
       <c r="D165" t="s">
-        <v>18</v>
+        <v>847</v>
       </c>
       <c r="E165" t="s">
-        <v>18</v>
+        <v>848</v>
       </c>
       <c r="F165" t="s">
         <v>18</v>
       </c>
       <c r="G165" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H165" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I165" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -7797,19 +8071,22 @@
         <v>441</v>
       </c>
       <c r="D166" t="s">
-        <v>18</v>
+        <v>849</v>
       </c>
       <c r="E166" t="s">
-        <v>18</v>
+        <v>850</v>
       </c>
       <c r="F166" t="s">
         <v>18</v>
       </c>
       <c r="G166" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H166" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I166" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -7823,19 +8100,22 @@
         <v>443</v>
       </c>
       <c r="D167" t="s">
-        <v>18</v>
+        <v>851</v>
       </c>
       <c r="E167" t="s">
-        <v>18</v>
+        <v>852</v>
       </c>
       <c r="F167" t="s">
         <v>18</v>
       </c>
       <c r="G167" t="s">
-        <v>18</v>
+        <v>564</v>
       </c>
       <c r="H167" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I167" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -7849,19 +8129,22 @@
         <v>445</v>
       </c>
       <c r="D168" t="s">
-        <v>18</v>
+        <v>853</v>
       </c>
       <c r="E168" t="s">
-        <v>18</v>
+        <v>854</v>
       </c>
       <c r="F168" t="s">
         <v>18</v>
       </c>
       <c r="G168" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H168" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I168" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -7875,19 +8158,22 @@
         <v>447</v>
       </c>
       <c r="D169" t="s">
-        <v>18</v>
+        <v>645</v>
       </c>
       <c r="E169" t="s">
-        <v>18</v>
+        <v>646</v>
       </c>
       <c r="F169" t="s">
         <v>18</v>
       </c>
       <c r="G169" t="s">
-        <v>18</v>
+        <v>624</v>
       </c>
       <c r="H169" t="s">
-        <v>18</v>
+        <v>145</v>
+      </c>
+      <c r="I169" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -7901,19 +8187,22 @@
         <v>449</v>
       </c>
       <c r="D170" t="s">
-        <v>18</v>
+        <v>857</v>
       </c>
       <c r="E170" t="s">
-        <v>18</v>
+        <v>858</v>
       </c>
       <c r="F170" t="s">
         <v>18</v>
       </c>
       <c r="G170" t="s">
-        <v>18</v>
+        <v>199</v>
       </c>
       <c r="H170" t="s">
-        <v>18</v>
+        <v>176</v>
+      </c>
+      <c r="I170" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -7927,19 +8216,22 @@
         <v>451</v>
       </c>
       <c r="D171" t="s">
-        <v>18</v>
+        <v>859</v>
       </c>
       <c r="E171" t="s">
-        <v>18</v>
+        <v>860</v>
       </c>
       <c r="F171" t="s">
         <v>18</v>
       </c>
       <c r="G171" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H171" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I171" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -7953,19 +8245,22 @@
         <v>453</v>
       </c>
       <c r="D172" t="s">
-        <v>18</v>
+        <v>861</v>
       </c>
       <c r="E172" t="s">
-        <v>18</v>
+        <v>862</v>
       </c>
       <c r="F172" t="s">
         <v>18</v>
       </c>
       <c r="G172" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H172" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I172" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -7979,19 +8274,22 @@
         <v>455</v>
       </c>
       <c r="D173" t="s">
-        <v>18</v>
+        <v>863</v>
       </c>
       <c r="E173" t="s">
-        <v>18</v>
+        <v>864</v>
       </c>
       <c r="F173" t="s">
         <v>18</v>
       </c>
       <c r="G173" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H173" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I173" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -8005,19 +8303,22 @@
         <v>457</v>
       </c>
       <c r="D174" t="s">
-        <v>18</v>
+        <v>865</v>
       </c>
       <c r="E174" t="s">
-        <v>18</v>
+        <v>866</v>
       </c>
       <c r="F174" t="s">
         <v>18</v>
       </c>
       <c r="G174" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H174" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I174" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -8031,19 +8332,22 @@
         <v>459</v>
       </c>
       <c r="D175" t="s">
-        <v>18</v>
+        <v>867</v>
       </c>
       <c r="E175" t="s">
-        <v>18</v>
+        <v>868</v>
       </c>
       <c r="F175" t="s">
         <v>18</v>
       </c>
       <c r="G175" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H175" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I175" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -8057,22 +8361,25 @@
         <v>461</v>
       </c>
       <c r="D176" t="s">
-        <v>18</v>
+        <v>869</v>
       </c>
       <c r="E176" t="s">
-        <v>18</v>
+        <v>870</v>
       </c>
       <c r="F176" t="s">
         <v>18</v>
       </c>
       <c r="G176" t="s">
-        <v>18</v>
+        <v>624</v>
       </c>
       <c r="H176" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="I176" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>462</v>
       </c>
@@ -8083,22 +8390,25 @@
         <v>463</v>
       </c>
       <c r="D177" t="s">
-        <v>18</v>
+        <v>871</v>
       </c>
       <c r="E177" t="s">
-        <v>18</v>
+        <v>872</v>
       </c>
       <c r="F177" t="s">
         <v>18</v>
       </c>
       <c r="G177" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H177" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I177" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>464</v>
       </c>
@@ -8123,8 +8433,11 @@
       <c r="H178" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>468</v>
       </c>
@@ -8135,22 +8448,25 @@
         <v>469</v>
       </c>
       <c r="D179" t="s">
-        <v>18</v>
+        <v>873</v>
       </c>
       <c r="E179" t="s">
-        <v>18</v>
+        <v>874</v>
       </c>
       <c r="F179" t="s">
         <v>18</v>
       </c>
       <c r="G179" t="s">
-        <v>18</v>
+        <v>875</v>
       </c>
       <c r="H179" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+      <c r="I179" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>470</v>
       </c>
@@ -8161,22 +8477,25 @@
         <v>471</v>
       </c>
       <c r="D180" t="s">
-        <v>18</v>
+        <v>876</v>
       </c>
       <c r="E180" t="s">
-        <v>18</v>
+        <v>877</v>
       </c>
       <c r="F180" t="s">
         <v>18</v>
       </c>
       <c r="G180" t="s">
-        <v>18</v>
+        <v>875</v>
       </c>
       <c r="H180" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+      <c r="I180" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>472</v>
       </c>
@@ -8187,22 +8506,25 @@
         <v>473</v>
       </c>
       <c r="D181" t="s">
-        <v>18</v>
+        <v>878</v>
       </c>
       <c r="E181" t="s">
-        <v>18</v>
+        <v>879</v>
       </c>
       <c r="F181" t="s">
         <v>18</v>
       </c>
       <c r="G181" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H181" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I181" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>474</v>
       </c>
@@ -8213,22 +8535,25 @@
         <v>475</v>
       </c>
       <c r="D182" t="s">
-        <v>18</v>
+        <v>880</v>
       </c>
       <c r="E182" t="s">
-        <v>18</v>
+        <v>881</v>
       </c>
       <c r="F182" t="s">
         <v>18</v>
       </c>
       <c r="G182" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H182" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I182" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>476</v>
       </c>
@@ -8239,22 +8564,25 @@
         <v>477</v>
       </c>
       <c r="D183" t="s">
-        <v>18</v>
+        <v>882</v>
       </c>
       <c r="E183" t="s">
-        <v>18</v>
+        <v>883</v>
       </c>
       <c r="F183" t="s">
         <v>18</v>
       </c>
       <c r="G183" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H183" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I183" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>478</v>
       </c>
@@ -8265,22 +8593,25 @@
         <v>479</v>
       </c>
       <c r="D184" t="s">
-        <v>18</v>
+        <v>884</v>
       </c>
       <c r="E184" t="s">
-        <v>18</v>
+        <v>885</v>
       </c>
       <c r="F184" t="s">
         <v>18</v>
       </c>
       <c r="G184" t="s">
-        <v>18</v>
+        <v>598</v>
       </c>
       <c r="H184" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="I184" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>480</v>
       </c>
@@ -8305,8 +8636,11 @@
       <c r="H185" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I185" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>484</v>
       </c>
@@ -8317,22 +8651,25 @@
         <v>485</v>
       </c>
       <c r="D186" t="s">
-        <v>18</v>
+        <v>886</v>
       </c>
       <c r="E186" t="s">
-        <v>18</v>
+        <v>887</v>
       </c>
       <c r="F186" t="s">
         <v>18</v>
       </c>
       <c r="G186" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="H186" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="I186" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>486</v>
       </c>
@@ -8357,8 +8694,11 @@
       <c r="H187" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I187" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>491</v>
       </c>
@@ -8369,22 +8709,25 @@
         <v>492</v>
       </c>
       <c r="D188" t="s">
-        <v>18</v>
+        <v>888</v>
       </c>
       <c r="E188" t="s">
-        <v>18</v>
+        <v>889</v>
       </c>
       <c r="F188" t="s">
         <v>18</v>
       </c>
       <c r="G188" t="s">
-        <v>18</v>
+        <v>199</v>
       </c>
       <c r="H188" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="I188" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>493</v>
       </c>
@@ -8395,22 +8738,25 @@
         <v>494</v>
       </c>
       <c r="D189" t="s">
-        <v>18</v>
+        <v>890</v>
       </c>
       <c r="E189" t="s">
-        <v>18</v>
+        <v>891</v>
       </c>
       <c r="F189" t="s">
         <v>18</v>
       </c>
       <c r="G189" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H189" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I189" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>495</v>
       </c>
@@ -8421,22 +8767,25 @@
         <v>496</v>
       </c>
       <c r="D190" t="s">
-        <v>18</v>
+        <v>892</v>
       </c>
       <c r="E190" t="s">
-        <v>18</v>
+        <v>893</v>
       </c>
       <c r="F190" t="s">
         <v>18</v>
       </c>
       <c r="G190" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H190" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I190" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>497</v>
       </c>
@@ -8459,10 +8808,16 @@
         <v>501</v>
       </c>
       <c r="H191" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+      <c r="I191" t="s">
+        <v>18</v>
+      </c>
+      <c r="J191" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>502</v>
       </c>
@@ -8473,22 +8828,25 @@
         <v>503</v>
       </c>
       <c r="D192" t="s">
-        <v>18</v>
+        <v>895</v>
       </c>
       <c r="E192" t="s">
-        <v>18</v>
+        <v>896</v>
       </c>
       <c r="F192" t="s">
         <v>18</v>
       </c>
       <c r="G192" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H192" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I192" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>504</v>
       </c>
@@ -8499,22 +8857,25 @@
         <v>505</v>
       </c>
       <c r="D193" t="s">
-        <v>18</v>
+        <v>897</v>
       </c>
       <c r="E193" t="s">
-        <v>18</v>
+        <v>898</v>
       </c>
       <c r="F193" t="s">
         <v>18</v>
       </c>
       <c r="G193" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H193" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I193" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>506</v>
       </c>
@@ -8525,22 +8886,25 @@
         <v>507</v>
       </c>
       <c r="D194" t="s">
-        <v>18</v>
+        <v>899</v>
       </c>
       <c r="E194" t="s">
-        <v>18</v>
+        <v>900</v>
       </c>
       <c r="F194" t="s">
         <v>18</v>
       </c>
       <c r="G194" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H194" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I194" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>508</v>
       </c>
@@ -8551,22 +8915,25 @@
         <v>509</v>
       </c>
       <c r="D195" t="s">
-        <v>18</v>
+        <v>901</v>
       </c>
       <c r="E195" t="s">
-        <v>18</v>
+        <v>902</v>
       </c>
       <c r="F195" t="s">
         <v>18</v>
       </c>
       <c r="G195" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H195" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I195" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>510</v>
       </c>
@@ -8577,22 +8944,25 @@
         <v>511</v>
       </c>
       <c r="D196" t="s">
-        <v>18</v>
+        <v>903</v>
       </c>
       <c r="E196" t="s">
-        <v>18</v>
+        <v>904</v>
       </c>
       <c r="F196" t="s">
         <v>18</v>
       </c>
       <c r="G196" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H196" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I196" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>512</v>
       </c>
@@ -8603,22 +8973,25 @@
         <v>513</v>
       </c>
       <c r="D197" t="s">
-        <v>18</v>
+        <v>905</v>
       </c>
       <c r="E197" t="s">
-        <v>18</v>
+        <v>906</v>
       </c>
       <c r="F197" t="s">
         <v>18</v>
       </c>
       <c r="G197" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H197" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I197" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>514</v>
       </c>
@@ -8629,22 +9002,25 @@
         <v>515</v>
       </c>
       <c r="D198" t="s">
-        <v>18</v>
+        <v>907</v>
       </c>
       <c r="E198" t="s">
-        <v>18</v>
+        <v>908</v>
       </c>
       <c r="F198" t="s">
         <v>18</v>
       </c>
       <c r="G198" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H198" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I198" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>516</v>
       </c>
@@ -8655,22 +9031,25 @@
         <v>517</v>
       </c>
       <c r="D199" t="s">
-        <v>18</v>
+        <v>909</v>
       </c>
       <c r="E199" t="s">
-        <v>18</v>
+        <v>910</v>
       </c>
       <c r="F199" t="s">
         <v>18</v>
       </c>
       <c r="G199" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H199" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I199" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>518</v>
       </c>
@@ -8681,22 +9060,25 @@
         <v>519</v>
       </c>
       <c r="D200" t="s">
-        <v>18</v>
+        <v>911</v>
       </c>
       <c r="E200" t="s">
-        <v>18</v>
+        <v>912</v>
       </c>
       <c r="F200" t="s">
         <v>18</v>
       </c>
       <c r="G200" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H200" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I200" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>520</v>
       </c>
@@ -8707,22 +9089,25 @@
         <v>521</v>
       </c>
       <c r="D201" t="s">
-        <v>18</v>
+        <v>913</v>
       </c>
       <c r="E201" t="s">
-        <v>18</v>
+        <v>914</v>
       </c>
       <c r="F201" t="s">
         <v>18</v>
       </c>
       <c r="G201" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H201" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I201" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>522</v>
       </c>
@@ -8733,22 +9118,25 @@
         <v>523</v>
       </c>
       <c r="D202" t="s">
-        <v>18</v>
+        <v>915</v>
       </c>
       <c r="E202" t="s">
-        <v>18</v>
+        <v>916</v>
       </c>
       <c r="F202" t="s">
         <v>18</v>
       </c>
       <c r="G202" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="H202" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="I202" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>524</v>
       </c>
@@ -8759,22 +9147,25 @@
         <v>525</v>
       </c>
       <c r="D203" t="s">
-        <v>18</v>
+        <v>917</v>
       </c>
       <c r="E203" t="s">
-        <v>18</v>
+        <v>918</v>
       </c>
       <c r="F203" t="s">
         <v>18</v>
       </c>
       <c r="G203" t="s">
-        <v>18</v>
+        <v>919</v>
       </c>
       <c r="H203" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I203" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>526</v>
       </c>
@@ -8785,22 +9176,25 @@
         <v>527</v>
       </c>
       <c r="D204" t="s">
-        <v>18</v>
+        <v>920</v>
       </c>
       <c r="E204" t="s">
-        <v>18</v>
+        <v>921</v>
       </c>
       <c r="F204" t="s">
         <v>18</v>
       </c>
       <c r="G204" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H204" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I204" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>528</v>
       </c>
@@ -8811,22 +9205,25 @@
         <v>529</v>
       </c>
       <c r="D205" t="s">
-        <v>18</v>
+        <v>922</v>
       </c>
       <c r="E205" t="s">
-        <v>18</v>
+        <v>923</v>
       </c>
       <c r="F205" t="s">
         <v>18</v>
       </c>
       <c r="G205" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H205" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I205" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>530</v>
       </c>
@@ -8837,22 +9234,25 @@
         <v>531</v>
       </c>
       <c r="D206" t="s">
-        <v>18</v>
+        <v>924</v>
       </c>
       <c r="E206" t="s">
-        <v>18</v>
+        <v>925</v>
       </c>
       <c r="F206" t="s">
         <v>18</v>
       </c>
       <c r="G206" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H206" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I206" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>532</v>
       </c>
@@ -8863,22 +9263,25 @@
         <v>533</v>
       </c>
       <c r="D207" t="s">
-        <v>18</v>
+        <v>926</v>
       </c>
       <c r="E207" t="s">
-        <v>18</v>
+        <v>927</v>
       </c>
       <c r="F207" t="s">
         <v>18</v>
       </c>
       <c r="G207" t="s">
-        <v>18</v>
+        <v>551</v>
       </c>
       <c r="H207" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I207" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>534</v>
       </c>
@@ -8889,19 +9292,22 @@
         <v>535</v>
       </c>
       <c r="D208" t="s">
-        <v>18</v>
+        <v>928</v>
       </c>
       <c r="E208" t="s">
-        <v>18</v>
+        <v>929</v>
       </c>
       <c r="F208" t="s">
         <v>18</v>
       </c>
       <c r="G208" t="s">
-        <v>18</v>
+        <v>875</v>
       </c>
       <c r="H208" t="s">
-        <v>18</v>
+        <v>465</v>
+      </c>
+      <c r="I208" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -8915,19 +9321,22 @@
         <v>537</v>
       </c>
       <c r="D209" t="s">
-        <v>18</v>
+        <v>930</v>
       </c>
       <c r="E209" t="s">
-        <v>18</v>
+        <v>931</v>
       </c>
       <c r="F209" t="s">
         <v>18</v>
       </c>
       <c r="G209" t="s">
-        <v>18</v>
+        <v>624</v>
       </c>
       <c r="H209" t="s">
-        <v>18</v>
+        <v>145</v>
+      </c>
+      <c r="I209" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -8941,19 +9350,22 @@
         <v>539</v>
       </c>
       <c r="D210" t="s">
-        <v>18</v>
+        <v>932</v>
       </c>
       <c r="E210" t="s">
-        <v>18</v>
+        <v>933</v>
       </c>
       <c r="F210" t="s">
         <v>18</v>
       </c>
       <c r="G210" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H210" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I210" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -8967,19 +9379,22 @@
         <v>541</v>
       </c>
       <c r="D211" t="s">
-        <v>18</v>
+        <v>934</v>
       </c>
       <c r="E211" t="s">
-        <v>18</v>
+        <v>935</v>
       </c>
       <c r="F211" t="s">
         <v>18</v>
       </c>
       <c r="G211" t="s">
-        <v>18</v>
+        <v>686</v>
       </c>
       <c r="H211" t="s">
-        <v>18</v>
+        <v>242</v>
+      </c>
+      <c r="I211" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -8993,19 +9408,22 @@
         <v>543</v>
       </c>
       <c r="D212" t="s">
-        <v>18</v>
+        <v>936</v>
       </c>
       <c r="E212" t="s">
-        <v>18</v>
+        <v>937</v>
       </c>
       <c r="F212" t="s">
         <v>18</v>
       </c>
       <c r="G212" t="s">
-        <v>18</v>
+        <v>199</v>
       </c>
       <c r="H212" t="s">
-        <v>18</v>
+        <v>176</v>
+      </c>
+      <c r="I212" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -9038,6 +9456,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J213" xr:uid="{AF803885-FA68-4431-A905-937B1B2D1406}"/>
   <hyperlinks>
     <hyperlink ref="D20" r:id="rId1" xr:uid="{22EB7AA0-1C51-45C3-ADB7-67918F3E3DB4}"/>
     <hyperlink ref="D30" r:id="rId2" xr:uid="{620B1651-FE43-4726-B429-9DF38AFE9E46}"/>

</xml_diff>

<commit_message>
fix country code for single university
</commit_message>
<xml_diff>
--- a/data/processed/leiden_matching_table.xlsx
+++ b/data/processed/leiden_matching_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tklebel\Documents\Projects\ON-MERRIT\03-Analysis\apc_effect\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E63B1B0-24E5-4734-A76B-02481A628C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9584A898-581D-40F5-90E8-27AE611A3443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16354" yWindow="7646" windowWidth="22149" windowHeight="12103" xr2:uid="{70655950-438C-47E9-B52C-924540BD7C84}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="939">
   <si>
     <t>University</t>
   </si>
@@ -2792,9 +2792,6 @@
   </si>
   <si>
     <t>University of the West of England</t>
-  </si>
-  <si>
-    <t>UK</t>
   </si>
   <si>
     <t>https://openalex.org/I201448701</t>
@@ -3247,8 +3244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF803885-FA68-4431-A905-937B1B2D1406}">
   <dimension ref="A1:J213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D188" sqref="D188"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G204" sqref="G204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,19 +3303,19 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>930</v>
+      </c>
+      <c r="E2" t="s">
         <v>931</v>
-      </c>
-      <c r="E2" t="s">
-        <v>932</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
+        <v>932</v>
+      </c>
+      <c r="H2" t="s">
         <v>933</v>
-      </c>
-      <c r="H2" t="s">
-        <v>934</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -3454,10 +3451,10 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
+        <v>934</v>
+      </c>
+      <c r="E7" t="s">
         <v>935</v>
-      </c>
-      <c r="E7" t="s">
-        <v>936</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -8686,16 +8683,16 @@
         <v>483</v>
       </c>
       <c r="D187" t="s">
+        <v>936</v>
+      </c>
+      <c r="E187" t="s">
         <v>937</v>
-      </c>
-      <c r="E187" t="s">
-        <v>938</v>
       </c>
       <c r="F187" t="s">
         <v>11</v>
       </c>
       <c r="G187" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="H187" t="s">
         <v>160</v>
@@ -9162,7 +9159,7 @@
         <v>15</v>
       </c>
       <c r="G203" t="s">
-        <v>912</v>
+        <v>561</v>
       </c>
       <c r="H203" t="s">
         <v>57</v>
@@ -9182,10 +9179,10 @@
         <v>520</v>
       </c>
       <c r="D204" t="s">
+        <v>912</v>
+      </c>
+      <c r="E204" t="s">
         <v>913</v>
-      </c>
-      <c r="E204" t="s">
-        <v>914</v>
       </c>
       <c r="F204" t="s">
         <v>15</v>
@@ -9211,10 +9208,10 @@
         <v>522</v>
       </c>
       <c r="D205" t="s">
+        <v>914</v>
+      </c>
+      <c r="E205" t="s">
         <v>915</v>
-      </c>
-      <c r="E205" t="s">
-        <v>916</v>
       </c>
       <c r="F205" t="s">
         <v>15</v>
@@ -9240,10 +9237,10 @@
         <v>524</v>
       </c>
       <c r="D206" t="s">
+        <v>916</v>
+      </c>
+      <c r="E206" t="s">
         <v>917</v>
-      </c>
-      <c r="E206" t="s">
-        <v>918</v>
       </c>
       <c r="F206" t="s">
         <v>15</v>
@@ -9269,10 +9266,10 @@
         <v>526</v>
       </c>
       <c r="D207" t="s">
+        <v>918</v>
+      </c>
+      <c r="E207" t="s">
         <v>919</v>
-      </c>
-      <c r="E207" t="s">
-        <v>920</v>
       </c>
       <c r="F207" t="s">
         <v>15</v>
@@ -9298,10 +9295,10 @@
         <v>528</v>
       </c>
       <c r="D208" t="s">
+        <v>920</v>
+      </c>
+      <c r="E208" t="s">
         <v>921</v>
-      </c>
-      <c r="E208" t="s">
-        <v>922</v>
       </c>
       <c r="F208" t="s">
         <v>15</v>
@@ -9327,10 +9324,10 @@
         <v>530</v>
       </c>
       <c r="D209" t="s">
+        <v>922</v>
+      </c>
+      <c r="E209" t="s">
         <v>923</v>
-      </c>
-      <c r="E209" t="s">
-        <v>924</v>
       </c>
       <c r="F209" t="s">
         <v>15</v>
@@ -9356,10 +9353,10 @@
         <v>532</v>
       </c>
       <c r="D210" t="s">
+        <v>924</v>
+      </c>
+      <c r="E210" t="s">
         <v>925</v>
-      </c>
-      <c r="E210" t="s">
-        <v>926</v>
       </c>
       <c r="F210" t="s">
         <v>15</v>
@@ -9385,10 +9382,10 @@
         <v>534</v>
       </c>
       <c r="D211" t="s">
+        <v>926</v>
+      </c>
+      <c r="E211" t="s">
         <v>927</v>
-      </c>
-      <c r="E211" t="s">
-        <v>928</v>
       </c>
       <c r="F211" t="s">
         <v>15</v>
@@ -9414,10 +9411,10 @@
         <v>536</v>
       </c>
       <c r="D212" t="s">
+        <v>928</v>
+      </c>
+      <c r="E212" t="s">
         <v>929</v>
-      </c>
-      <c r="E212" t="s">
-        <v>930</v>
       </c>
       <c r="F212" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
forgot to add the correct country identifier
</commit_message>
<xml_diff>
--- a/data/processed/leiden_matching_table.xlsx
+++ b/data/processed/leiden_matching_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tklebel\Documents\Projects\ON-MERRIT\03-Analysis\apc_effect\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98394331-4805-48B1-AA11-56C584235D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2405B138-DF96-4BD2-BBE9-776E46324D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" xr2:uid="{70655950-438C-47E9-B52C-924540BD7C84}"/>
   </bookViews>
@@ -3248,7 +3248,7 @@
   <dimension ref="A1:J213"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4484,7 +4484,7 @@
         <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="H42" t="s">
         <v>43</v>

</xml_diff>